<commit_message>
Docs Auxiliares queries, contabilidade e compras
</commit_message>
<xml_diff>
--- a/DocsAux/queries_modulos.xlsx
+++ b/DocsAux/queries_modulos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Querie 1</t>
   </si>
@@ -81,13 +81,76 @@
   </si>
   <si>
     <t>Catálogo</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Letra</t>
+  </si>
+  <si>
+    <t>Lista e total produtos</t>
+  </si>
+  <si>
+    <t>Cod. Produto + Mes</t>
+  </si>
+  <si>
+    <t>Nº Vendas + Total facturado</t>
+  </si>
+  <si>
+    <t>Lista e nº produtos com 0 vendas</t>
+  </si>
+  <si>
+    <t>Cod. Cliente</t>
+  </si>
+  <si>
+    <t>Nº prods comprados mês a mês</t>
+  </si>
+  <si>
+    <t>Lista e total clientes</t>
+  </si>
+  <si>
+    <t>Intervalo Meses</t>
+  </si>
+  <si>
+    <t>Nº compras e total facturado</t>
+  </si>
+  <si>
+    <t>Cod. Produto</t>
+  </si>
+  <si>
+    <t>Lista de clientes que compraram</t>
+  </si>
+  <si>
+    <t>Cod. Cliente + Mes</t>
+  </si>
+  <si>
+    <t>Produtos mais comprados (lista)</t>
+  </si>
+  <si>
+    <t>Cod. Clientes regulares</t>
+  </si>
+  <si>
+    <t>Nº Compras e Nº Clientes (CSV)</t>
+  </si>
+  <si>
+    <t>N Produtos mais vendidos</t>
+  </si>
+  <si>
+    <t>3 produtos mais comprados</t>
+  </si>
+  <si>
+    <t>Clientes e Produtos "zombie"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +166,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -136,21 +218,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -192,57 +259,247 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -253,84 +510,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -340,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,61 +527,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,177 +897,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="4" max="8" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="20"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="20"/>
-    </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="20"/>
-    </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="B14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Queries incompletas acabadas + melhorias interface
</commit_message>
<xml_diff>
--- a/DocsAux/queries_modulos.xlsx
+++ b/DocsAux/queries_modulos.xlsx
@@ -626,7 +626,7 @@
   <dimension ref="A1:XFD15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17220,7 +17220,7 @@
       <c r="D13" s="27"/>
       <c r="E13" s="28"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:16384" ht="20.1" customHeight="1">

</xml_diff>

<commit_message>
Arvore nº clientes nas compras
</commit_message>
<xml_diff>
--- a/DocsAux/queries_modulos.xlsx
+++ b/DocsAux/queries_modulos.xlsx
@@ -19,21 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
   <si>
-    <t>500k</t>
-  </si>
-  <si>
-    <t>1m</t>
-  </si>
-  <si>
-    <t>3m</t>
+    <t>LEITURA</t>
   </si>
   <si>
     <t>LEITURA</t>
   </si>
   <si>
     <t>Letra</t>
+  </si>
+  <si>
+    <t>Nenhuma a assinalar</t>
   </si>
   <si>
     <t>Cod. Cliente</t>
@@ -856,13 +853,13 @@
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="14" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="15" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="31" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="4" borderId="26" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
@@ -895,13 +892,13 @@
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="16" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="18" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="32" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
@@ -958,13 +955,13 @@
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="41" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="42" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="43" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -978,7 +975,7 @@
   <dimension ref="A1:XFD16"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
-      <selection activeCell="L5" sqref="L5:N5"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -990,7 +987,8 @@
     <col min="9" max="11" style="1" width="11.42788" customWidth="1"/>
     <col min="12" max="12" style="1" width="12.9516" customWidth="1"/>
     <col min="13" max="13" style="1" width="11.99928" customWidth="1"/>
-    <col min="14" max="16384" style="1" width="9.140625"/>
+    <col min="14" max="14" style="1" width="15.99904" customWidth="1"/>
+    <col min="15" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" ht="39.75" customHeight="1">
@@ -17406,14 +17404,14 @@
       <c r="F2" s="6"/>
       <c r="G2" s="4"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="15" t="s">
-        <v>0</v>
+      <c r="I2" s="15" t="str">
+        <v>500k</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>1</v>
+      <c r="J2" s="16" t="str">
+        <v>1m</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>2</v>
+      <c r="K2" s="16" t="str">
+        <v>3m</v>
       </c>
       <c r="L2" s="17"/>
       <c r="M2" s="18"/>
@@ -33794,11 +33792,11 @@
         <v>Querie 1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="23" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
@@ -33816,7 +33814,7 @@
         <v>Querie 2</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="32" t="str">
         <v>Lista e total produtos</v>
@@ -33831,8 +33829,8 @@
         <v>0.00238</v>
       </c>
       <c r="K4" s="39"/>
-      <c r="L4" s="40" t="str">
-        <v>Nenhuma a assinalar</v>
+      <c r="L4" s="40" t="s">
+        <v>3</v>
       </c>
       <c r="M4" s="41"/>
       <c r="N4" s="42"/>
@@ -33853,9 +33851,13 @@
       <c r="G5" s="49"/>
       <c r="H5" s="50"/>
       <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="J5" s="52">
+        <v>4e-05</v>
+      </c>
       <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
+      <c r="L5" s="53" t="s">
+        <v>3</v>
+      </c>
       <c r="M5" s="54"/>
       <c r="N5" s="55"/>
     </row>
@@ -33873,9 +33875,13 @@
       <c r="G6" s="49"/>
       <c r="H6" s="50"/>
       <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
+      <c r="J6" s="52">
+        <v>0.01925</v>
+      </c>
       <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="L6" s="53" t="str">
+        <v>Clone da ficha completo</v>
+      </c>
       <c r="M6" s="54"/>
       <c r="N6" s="55"/>
     </row>
@@ -33884,7 +33890,7 @@
         <v>Querie 5</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="57" t="str">
         <v>Nº prods comprados mês a mês + fich</v>
@@ -33895,9 +33901,13 @@
       <c r="G7" s="60"/>
       <c r="H7" s="61"/>
       <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
+      <c r="J7" s="52">
+        <v>4e-05</v>
+      </c>
       <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
+      <c r="L7" s="53" t="s">
+        <v>3</v>
+      </c>
       <c r="M7" s="54"/>
       <c r="N7" s="55"/>
     </row>
@@ -33906,7 +33916,7 @@
         <v>Querie 6</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="57" t="str">
         <v>Lista e total clientes</v>
@@ -33917,9 +33927,13 @@
       <c r="G8" s="63"/>
       <c r="H8" s="61"/>
       <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="J8" s="52">
+        <v>0.00068</v>
+      </c>
       <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
+      <c r="L8" s="53" t="s">
+        <v>3</v>
+      </c>
       <c r="M8" s="54"/>
       <c r="N8" s="55"/>
     </row>
@@ -33939,9 +33953,13 @@
       <c r="G9" s="49"/>
       <c r="H9" s="50"/>
       <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
+      <c r="J9" s="52">
+        <v>0.00013</v>
+      </c>
       <c r="K9" s="52"/>
-      <c r="L9" s="53"/>
+      <c r="L9" s="53" t="str">
+        <v>Eliminar chamadas repetidas ao modulo</v>
+      </c>
       <c r="M9" s="54"/>
       <c r="N9" s="55"/>
     </row>
@@ -33961,9 +33979,13 @@
       <c r="G10" s="60"/>
       <c r="H10" s="50"/>
       <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
+      <c r="J10" s="52">
+        <v>0.0279</v>
+      </c>
       <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
+      <c r="L10" s="53" t="s">
+        <v>3</v>
+      </c>
       <c r="M10" s="54"/>
       <c r="N10" s="55"/>
     </row>
@@ -33983,9 +34005,13 @@
       <c r="G11" s="60"/>
       <c r="H11" s="61"/>
       <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
+      <c r="J11" s="52">
+        <v>7e-05</v>
+      </c>
       <c r="K11" s="52"/>
-      <c r="L11" s="53"/>
+      <c r="L11" s="53" t="s">
+        <v>3</v>
+      </c>
       <c r="M11" s="54"/>
       <c r="N11" s="55"/>
     </row>
@@ -34003,7 +34029,9 @@
       <c r="G12" s="60"/>
       <c r="H12" s="61"/>
       <c r="I12" s="51"/>
-      <c r="J12" s="52"/>
+      <c r="J12" s="52">
+        <v>0.00623</v>
+      </c>
       <c r="K12" s="52"/>
       <c r="L12" s="53"/>
       <c r="M12" s="54"/>
@@ -34023,7 +34051,9 @@
       <c r="G13" s="60"/>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
+      <c r="J13" s="52">
+        <v>0.0024</v>
+      </c>
       <c r="K13" s="52"/>
       <c r="L13" s="53"/>
       <c r="M13" s="54"/>
@@ -34054,7 +34084,7 @@
         <v>Querie 13</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="57" t="str">
         <v>3 produtos mais comprados</v>
@@ -34065,7 +34095,9 @@
       <c r="G15" s="60"/>
       <c r="H15" s="61"/>
       <c r="I15" s="51"/>
-      <c r="J15" s="52"/>
+      <c r="J15" s="52">
+        <v>3e-05</v>
+      </c>
       <c r="K15" s="52"/>
       <c r="L15" s="53"/>
       <c r="M15" s="54"/>
@@ -34085,7 +34117,9 @@
       <c r="G16" s="70"/>
       <c r="H16" s="71"/>
       <c r="I16" s="72"/>
-      <c r="J16" s="73"/>
+      <c r="J16" s="73">
+        <v>0.02284</v>
+      </c>
       <c r="K16" s="73"/>
       <c r="L16" s="74"/>
       <c r="M16" s="75"/>

</xml_diff>

<commit_message>
Corrigido leak de memoria nas arvores dos produtos das compras e correcção às funções de remoção
</commit_message>
<xml_diff>
--- a/DocsAux/queries_modulos.xlsx
+++ b/DocsAux/queries_modulos.xlsx
@@ -115,17 +115,17 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
-    <border diagonalUp="0" diagonalDown="0">
+  <borders count="42">
+    <border diagonalDown="0">
+      <left style="none">
+        <color rgb="FFC7C7C7"/>
+      </left>
       <right style="none">
         <color rgb="FFC7C7C7"/>
       </right>
       <top style="none">
         <color rgb="FFC7C7C7"/>
       </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
       <left style="none">
@@ -408,20 +408,6 @@
       </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
@@ -455,20 +441,6 @@
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
       </right>
       <top style="thick">
         <color rgb="FF000000"/>
@@ -733,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
@@ -798,8 +770,11 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="2" borderId="20" numFmtId="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="2" borderId="21" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="2" borderId="9" numFmtId="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="21" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="22" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
@@ -807,43 +782,37 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="23" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="24" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="25" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="9" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="8" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="9" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="10" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="26" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="24" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="25" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="28" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="26" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="25" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="27" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="27" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="29" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="29" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="26" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="28" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="30" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="14" numFmtId="100" xfId="0">
@@ -858,31 +827,31 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="15" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="31" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="29" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="4" borderId="26" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="4" borderId="24" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="4" borderId="32" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="4" borderId="30" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="4" borderId="33" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="4" borderId="31" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="30" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="32" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="34" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="32" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="34" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="31" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="33" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="35" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="16" numFmtId="100" xfId="0">
@@ -900,67 +869,67 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="32" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="30" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="33" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="31" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="30" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="32" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="34" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="31" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="33" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="33" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="30" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="31" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="34" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="35" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="36" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="35" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="32" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="33" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="36" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="37" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="5" fillId="0" borderId="38" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="37" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="39" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="37" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="39" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="36" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="38" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="38" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="40" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="39" numFmtId="100" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="41" numFmtId="100" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="40" numFmtId="100" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="42" numFmtId="100" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="39" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="40" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="41" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="42" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="43" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
@@ -975,7 +944,7 @@
   <dimension ref="A1:XFD16"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J10" sqref="A10:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33803,327 +33772,329 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
       <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A4" s="30" t="str">
+      <c r="A4" s="29" t="str">
         <v>Querie 2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32" t="str">
+      <c r="C4" s="31" t="str">
         <v>Lista e total produtos</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39">
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38">
         <v>0.00238</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40" t="s">
+      <c r="K4" s="38"/>
+      <c r="L4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="41"/>
-      <c r="N4" s="42"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A5" s="43" t="str">
+      <c r="A5" s="42" t="str">
         <v>Querie 3</v>
       </c>
-      <c r="B5" s="44" t="str">
+      <c r="B5" s="43" t="str">
         <v>Cod. Produto + Mes</v>
       </c>
-      <c r="C5" s="45" t="str">
+      <c r="C5" s="44" t="str">
         <v>Nº Vendas + Total facturado</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52">
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51">
         <v>4e-05</v>
       </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53" t="s">
+      <c r="K5" s="51"/>
+      <c r="L5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="54"/>
-      <c r="N5" s="55"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
     </row>
     <row r="6" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A6" s="43" t="str">
+      <c r="A6" s="42" t="str">
         <v>Querie 4</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45" t="str">
+      <c r="B6" s="43"/>
+      <c r="C6" s="44" t="str">
         <v>Lista e nº produtos com 0 vendas</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52">
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51">
         <v>0.01925</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53" t="str">
+      <c r="K6" s="51"/>
+      <c r="L6" s="52" t="str">
         <v>Clone da ficha completo</v>
       </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="55"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
     </row>
     <row r="7" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A7" s="30" t="str">
+      <c r="A7" s="29" t="str">
         <v>Querie 5</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="57" t="str">
+      <c r="C7" s="56" t="str">
         <v>Nº prods comprados mês a mês + fich</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52">
+      <c r="D7" s="57"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51">
         <v>4e-05</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53" t="s">
+      <c r="K7" s="51"/>
+      <c r="L7" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="54"/>
     </row>
     <row r="8" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A8" s="30" t="str">
+      <c r="A8" s="29" t="str">
         <v>Querie 6</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="57" t="str">
+      <c r="C8" s="56" t="str">
         <v>Lista e total clientes</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52">
+      <c r="D8" s="61"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="51">
         <v>0.00068</v>
       </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53" t="s">
+      <c r="K8" s="51"/>
+      <c r="L8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="54"/>
-      <c r="N8" s="55"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="54"/>
     </row>
     <row r="9" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A9" s="43" t="str">
+      <c r="A9" s="42" t="str">
         <v>Querie 7</v>
       </c>
-      <c r="B9" s="44" t="str">
+      <c r="B9" s="43" t="str">
         <v>Intervalo Meses</v>
       </c>
-      <c r="C9" s="45" t="str">
+      <c r="C9" s="44" t="str">
         <v>Nº compras e total facturado</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52">
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="51">
         <v>0.00013</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="53" t="str">
+      <c r="K9" s="51"/>
+      <c r="L9" s="52" t="str">
         <v>Eliminar chamadas repetidas ao modulo</v>
       </c>
-      <c r="M9" s="54"/>
-      <c r="N9" s="55"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="54"/>
     </row>
     <row r="10" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A10" s="43" t="str">
+      <c r="A10" s="42" t="str">
         <v>Querie 8</v>
       </c>
-      <c r="B10" s="44" t="str">
+      <c r="B10" s="43" t="str">
         <v>Cod. Produto</v>
       </c>
-      <c r="C10" s="45" t="str">
+      <c r="C10" s="44" t="str">
         <v>Lista de clientes que compraram (N e P)</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52">
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="51">
         <v>0.0279</v>
       </c>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53" t="s">
+      <c r="K10" s="51"/>
+      <c r="L10" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="54"/>
-      <c r="N10" s="55"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A11" s="30" t="str">
+      <c r="A11" s="29" t="str">
         <v>Querie 9</v>
       </c>
-      <c r="B11" s="56" t="str">
+      <c r="B11" s="55" t="str">
         <v>Cod. Cliente + Mes</v>
       </c>
-      <c r="C11" s="57" t="str">
+      <c r="C11" s="56" t="str">
         <v>Produtos mais comprados (lista)</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52">
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51">
         <v>7e-05</v>
       </c>
-      <c r="K11" s="52"/>
-      <c r="L11" s="53" t="s">
+      <c r="K11" s="51"/>
+      <c r="L11" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="54"/>
-      <c r="N11" s="55"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="54"/>
     </row>
     <row r="12" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="29" t="str">
         <v>Querie 10</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57" t="str">
+      <c r="B12" s="55"/>
+      <c r="C12" s="56" t="str">
         <v>Cod. Clientes regulares</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52">
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51">
         <v>0.00623</v>
       </c>
-      <c r="K12" s="52"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="55"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="54"/>
     </row>
     <row r="13" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A13" s="43" t="str">
+      <c r="A13" s="42" t="str">
         <v>Querie 11</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45" t="str">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="str">
         <v>Nº Compras e Nº Clientes (CSV)</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52">
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="51">
         <v>0.0024</v>
       </c>
-      <c r="K13" s="52"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="55"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="54"/>
     </row>
     <row r="14" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A14" s="43" t="str">
+      <c r="A14" s="42" t="str">
         <v>Querie 12</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45" t="str">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="str">
         <v>N Produtos mais vendidos</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="55"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="K14" s="51"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="54"/>
     </row>
     <row r="15" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="29" t="str">
         <v>Querie 13</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="57" t="str">
+      <c r="C15" s="56" t="str">
         <v>3 produtos mais comprados</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="52">
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51">
         <v>3e-05</v>
       </c>
-      <c r="K15" s="52"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="55"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="54"/>
     </row>
     <row r="16" spans="1:16384" ht="20.1" customHeight="1">
-      <c r="A16" s="64" t="str">
+      <c r="A16" s="63" t="str">
         <v>Querie 14</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66" t="str">
+      <c r="B16" s="64"/>
+      <c r="C16" s="65" t="str">
         <v>Clientes e Produtos "zombie"</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="73">
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="72">
         <v>0.02284</v>
       </c>
-      <c r="K16" s="73"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="76"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="75"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>